<commit_message>
Chỉnh sửa model Product, xóa bảng Price, Seed lại data
</commit_message>
<xml_diff>
--- a/DataExample/categories.xlsx
+++ b/DataExample/categories.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -400,127 +397,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>